<commit_message>
[UI] Material Option UI 정리 & Cost Option UI 작업
</commit_message>
<xml_diff>
--- a/DataTable/AdventureLevelTable.xlsx
+++ b/DataTable/AdventureLevelTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seh00n/GitHub/ProjectF/DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6D4F82E5-C482-454A-90AA-3407F8A34900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E6262589-1A51-314B-BCC0-E338F5574AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="4640" windowWidth="28300" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="3280" windowWidth="28300" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdventureLevelTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="360" uniqueCount="49">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="360" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -156,38 +156,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>70000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>500000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>3500000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>24500000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>171500000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1200500000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>8500000000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>60000000000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>20000</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -219,6 +187,9 @@
   <si>
     <t>600</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000</t>
   </si>
 </sst>
 </file>
@@ -1205,8 +1176,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1228,7 +1199,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -1270,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -1292,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1301,7 +1272,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -1314,13 +1285,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>11</v>
@@ -1336,13 +1307,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>28</v>
@@ -1358,13 +1329,13 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D8" s="4">
         <v>4</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>27</v>
@@ -1380,13 +1351,13 @@
         <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D9" s="4">
         <v>5</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>26</v>
@@ -1402,13 +1373,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D10" s="4">
         <v>6</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>25</v>
@@ -1424,13 +1395,13 @@
         <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D11" s="4">
         <v>7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>24</v>
@@ -1446,13 +1417,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4">
         <v>8</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>23</v>
@@ -1468,13 +1439,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D13" s="4">
         <v>9</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>22</v>
@@ -1490,13 +1461,13 @@
         <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F14" s="4">
         <v>400</v>
@@ -1512,16 +1483,16 @@
         <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -1534,16 +1505,16 @@
         <v>8</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D16" s="4">
         <v>2</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -1556,16 +1527,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D17" s="4">
         <v>3</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -1578,16 +1549,16 @@
         <v>8</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D18" s="4">
         <v>4</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -1600,16 +1571,16 @@
         <v>8</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D19" s="4">
         <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G19" s="3"/>
     </row>
@@ -1622,16 +1593,16 @@
         <v>8</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D20" s="4">
         <v>6</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G20" s="3"/>
     </row>
@@ -1644,16 +1615,16 @@
         <v>8</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D21" s="4">
         <v>7</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G21" s="3"/>
     </row>
@@ -1666,16 +1637,16 @@
         <v>8</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D22" s="4">
         <v>8</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G22" s="3"/>
     </row>
@@ -1688,16 +1659,16 @@
         <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D23" s="4">
         <v>9</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G23" s="3"/>
     </row>
@@ -1710,16 +1681,16 @@
         <v>13</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D24" s="4">
         <v>0</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G24" s="3"/>
     </row>
@@ -1732,16 +1703,16 @@
         <v>13</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G25" s="3"/>
     </row>
@@ -1754,16 +1725,16 @@
         <v>12</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D26" s="4">
         <v>2</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G26" s="3"/>
     </row>
@@ -1776,16 +1747,16 @@
         <v>12</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D27" s="4">
         <v>3</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G27" s="3"/>
     </row>
@@ -1798,16 +1769,16 @@
         <v>12</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D28" s="4">
         <v>4</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G28" s="3"/>
     </row>
@@ -1820,16 +1791,16 @@
         <v>12</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D29" s="4">
         <v>5</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G29" s="3"/>
     </row>
@@ -1842,16 +1813,16 @@
         <v>12</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D30" s="4">
         <v>6</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -1864,16 +1835,16 @@
         <v>12</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D31" s="4">
         <v>7</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G31" s="3"/>
     </row>
@@ -1886,16 +1857,16 @@
         <v>12</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D32" s="4">
         <v>8</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G32" s="3"/>
     </row>
@@ -1908,16 +1879,16 @@
         <v>12</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D33" s="4">
         <v>9</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G33" s="3"/>
     </row>
@@ -1930,16 +1901,16 @@
         <v>19</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D34" s="4">
         <v>0</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -1952,16 +1923,16 @@
         <v>19</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D35" s="4">
         <v>1</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G35" s="3"/>
     </row>
@@ -1974,16 +1945,16 @@
         <v>18</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D36" s="4">
         <v>2</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G36" s="3"/>
     </row>
@@ -1996,16 +1967,16 @@
         <v>18</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D37" s="4">
         <v>3</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G37" s="3"/>
     </row>
@@ -2018,16 +1989,16 @@
         <v>18</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D38" s="4">
         <v>4</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G38" s="3"/>
     </row>
@@ -2040,16 +2011,16 @@
         <v>18</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D39" s="4">
         <v>5</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G39" s="3"/>
     </row>
@@ -2062,16 +2033,16 @@
         <v>18</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D40" s="4">
         <v>6</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G40" s="3"/>
     </row>
@@ -2084,16 +2055,16 @@
         <v>18</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D41" s="4">
         <v>7</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G41" s="3"/>
     </row>
@@ -2106,16 +2077,16 @@
         <v>18</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D42" s="4">
         <v>8</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G42" s="3"/>
     </row>
@@ -2128,16 +2099,16 @@
         <v>18</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D43" s="4">
         <v>9</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G43" s="3"/>
     </row>
@@ -2150,16 +2121,16 @@
         <v>15</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D44" s="4">
         <v>0</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G44" s="3"/>
     </row>
@@ -2172,16 +2143,16 @@
         <v>15</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D45" s="4">
         <v>1</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G45" s="3"/>
     </row>
@@ -2194,16 +2165,16 @@
         <v>14</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D46" s="4">
         <v>2</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G46" s="3"/>
     </row>
@@ -2216,16 +2187,16 @@
         <v>14</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D47" s="4">
         <v>3</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G47" s="3"/>
     </row>
@@ -2238,16 +2209,16 @@
         <v>14</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D48" s="4">
         <v>4</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G48" s="3"/>
     </row>
@@ -2260,16 +2231,16 @@
         <v>14</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D49" s="4">
         <v>5</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G49" s="3"/>
     </row>
@@ -2282,16 +2253,16 @@
         <v>14</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D50" s="4">
         <v>6</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G50" s="3"/>
     </row>
@@ -2304,16 +2275,16 @@
         <v>14</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D51" s="4">
         <v>7</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G51" s="3"/>
     </row>
@@ -2326,16 +2297,16 @@
         <v>14</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D52" s="4">
         <v>8</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G52" s="3"/>
     </row>
@@ -2348,16 +2319,16 @@
         <v>14</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D53" s="4">
         <v>9</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G53" s="3"/>
     </row>
@@ -2370,16 +2341,16 @@
         <v>11</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D54" s="4">
         <v>0</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G54" s="3"/>
     </row>
@@ -2392,16 +2363,16 @@
         <v>11</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D55" s="4">
         <v>1</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G55" s="3"/>
     </row>
@@ -2414,16 +2385,16 @@
         <v>10</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D56" s="4">
         <v>2</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G56" s="3"/>
     </row>
@@ -2436,16 +2407,16 @@
         <v>10</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D57" s="4">
         <v>3</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G57" s="3"/>
     </row>
@@ -2458,16 +2429,16 @@
         <v>10</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D58" s="4">
         <v>4</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G58" s="3"/>
     </row>
@@ -2480,16 +2451,16 @@
         <v>10</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D59" s="4">
         <v>5</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G59" s="3"/>
     </row>
@@ -2502,16 +2473,16 @@
         <v>10</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D60" s="4">
         <v>6</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G60" s="3"/>
     </row>
@@ -2524,16 +2495,16 @@
         <v>10</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D61" s="4">
         <v>7</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G61" s="3"/>
     </row>
@@ -2546,16 +2517,16 @@
         <v>10</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D62" s="4">
         <v>8</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G62" s="3"/>
     </row>
@@ -2568,16 +2539,16 @@
         <v>10</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D63" s="4">
         <v>9</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G63" s="3"/>
     </row>
@@ -2590,16 +2561,16 @@
         <v>21</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D64" s="4">
         <v>0</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G64" s="3"/>
     </row>
@@ -2612,16 +2583,16 @@
         <v>21</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D65" s="4">
         <v>1</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G65" s="3"/>
     </row>
@@ -2634,16 +2605,16 @@
         <v>20</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D66" s="4">
         <v>2</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G66" s="3"/>
     </row>
@@ -2656,16 +2627,16 @@
         <v>20</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D67" s="4">
         <v>3</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G67" s="3"/>
     </row>
@@ -2678,16 +2649,16 @@
         <v>20</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D68" s="4">
         <v>4</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G68" s="3"/>
     </row>
@@ -2700,16 +2671,16 @@
         <v>20</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D69" s="4">
         <v>5</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G69" s="3"/>
     </row>
@@ -2722,16 +2693,16 @@
         <v>20</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D70" s="4">
         <v>6</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G70" s="3"/>
     </row>
@@ -2744,16 +2715,16 @@
         <v>20</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D71" s="4">
         <v>7</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G71" s="3"/>
     </row>
@@ -2766,16 +2737,16 @@
         <v>20</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D72" s="4">
         <v>8</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G72" s="3"/>
     </row>
@@ -2788,16 +2759,16 @@
         <v>20</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D73" s="4">
         <v>9</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G73" s="3"/>
     </row>
@@ -2810,16 +2781,16 @@
         <v>30</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D74" s="4">
         <v>0</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G74" s="3"/>
     </row>
@@ -2832,16 +2803,16 @@
         <v>30</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D75" s="4">
         <v>1</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G75" s="3"/>
     </row>
@@ -2854,16 +2825,16 @@
         <v>29</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D76" s="4">
         <v>2</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G76" s="3"/>
     </row>
@@ -2876,16 +2847,16 @@
         <v>29</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D77" s="4">
         <v>3</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G77" s="3"/>
     </row>
@@ -2898,16 +2869,16 @@
         <v>29</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D78" s="4">
         <v>4</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G78" s="3"/>
     </row>
@@ -2920,16 +2891,16 @@
         <v>29</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D79" s="4">
         <v>5</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G79" s="3"/>
     </row>
@@ -2942,16 +2913,16 @@
         <v>29</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D80" s="4">
         <v>6</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G80" s="3"/>
     </row>
@@ -2964,16 +2935,16 @@
         <v>29</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D81" s="4">
         <v>7</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G81" s="3"/>
     </row>
@@ -2986,16 +2957,16 @@
         <v>29</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D82" s="4">
         <v>8</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G82" s="3"/>
     </row>
@@ -3008,16 +2979,16 @@
         <v>29</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D83" s="4">
         <v>9</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G83" s="3"/>
     </row>
@@ -3030,16 +3001,16 @@
         <v>17</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D84" s="4">
         <v>0</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G84" s="3"/>
     </row>
@@ -3052,16 +3023,16 @@
         <v>17</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D85" s="4">
         <v>1</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G85" s="3"/>
     </row>
@@ -3074,16 +3045,16 @@
         <v>16</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D86" s="4">
         <v>2</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G86" s="3"/>
     </row>
@@ -3096,16 +3067,16 @@
         <v>16</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D87" s="4">
         <v>3</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G87" s="3"/>
     </row>
@@ -3118,16 +3089,16 @@
         <v>16</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D88" s="4">
         <v>4</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G88" s="3"/>
     </row>
@@ -3140,16 +3111,16 @@
         <v>16</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D89" s="4">
         <v>5</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G89" s="3"/>
     </row>
@@ -3162,16 +3133,16 @@
         <v>16</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D90" s="4">
         <v>6</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G90" s="3"/>
     </row>
@@ -3184,16 +3155,16 @@
         <v>16</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D91" s="4">
         <v>7</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G91" s="3"/>
     </row>
@@ -3206,16 +3177,16 @@
         <v>16</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D92" s="4">
         <v>8</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G92" s="3"/>
     </row>
@@ -3228,16 +3199,16 @@
         <v>16</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D93" s="4">
         <v>9</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G93" s="3"/>
     </row>

</xml_diff>